<commit_message>
uploading changes in data
</commit_message>
<xml_diff>
--- a/data/clean/aspen_meadow.xlsx
+++ b/data/clean/aspen_meadow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E56FB9-CDE1-4174-ADCB-C38262B2D4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F469D9-A80E-43DD-8CF4-D01A2EF0999B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Ground Cover" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>Shrubs</t>
   </si>
@@ -63,27 +63,6 @@
     <t>Dist meters</t>
   </si>
   <si>
-    <t>Tree 1</t>
-  </si>
-  <si>
-    <t>Tree 2</t>
-  </si>
-  <si>
-    <t>Tree 3</t>
-  </si>
-  <si>
-    <t>Tree 4</t>
-  </si>
-  <si>
-    <t>Distance (cm)</t>
-  </si>
-  <si>
-    <t>Circumfrence (cm)</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
     <t>AS</t>
   </si>
   <si>
@@ -121,6 +100,69 @@
   </si>
   <si>
     <t>Baby Trees</t>
+  </si>
+  <si>
+    <t>T1-Distance (cm)</t>
+  </si>
+  <si>
+    <t>T2-Circumfrence (cm)</t>
+  </si>
+  <si>
+    <t>T1-Circumfrence (cm)</t>
+  </si>
+  <si>
+    <t>T1-Species</t>
+  </si>
+  <si>
+    <t>T2-Distance (cm)</t>
+  </si>
+  <si>
+    <t>T2-Species</t>
+  </si>
+  <si>
+    <t>T3-Distance (cm)</t>
+  </si>
+  <si>
+    <t>T3-Circumfrence (cm)</t>
+  </si>
+  <si>
+    <t>T3-Species</t>
+  </si>
+  <si>
+    <t>T4-Distance (cm)</t>
+  </si>
+  <si>
+    <t>T4-Circumfrence (cm)</t>
+  </si>
+  <si>
+    <t>T4-Species</t>
+  </si>
+  <si>
+    <t>Note: added other column to ensure percentages were accounted for</t>
+  </si>
+  <si>
+    <t>Note: I believe we are missing the litter category for all the data sheets</t>
+  </si>
+  <si>
+    <t>T1-Tree 1</t>
+  </si>
+  <si>
+    <t>T2-Tree 2</t>
+  </si>
+  <si>
+    <t>T3-Tree 3</t>
+  </si>
+  <si>
+    <t>T4-Tree 4</t>
+  </si>
+  <si>
+    <t>Note : 2024 calculations did not include the unaccounted for 20% in transect 2</t>
+  </si>
+  <si>
+    <t>AS-aspen</t>
+  </si>
+  <si>
+    <t>LP-lodgepole pine</t>
   </si>
 </sst>
 </file>
@@ -130,18 +172,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
     </font>
     <font>
       <sz val="11"/>
@@ -170,14 +207,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,13 +492,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
@@ -474,16 +511,16 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -527,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" ref="J2:J11" si="0">SUM(C2+D2+E2+F2+G2+H2+I2)</f>
+        <f>SUM(C2+D2+E2+F2+G2+H2+I2)</f>
         <v>100</v>
       </c>
     </row>
@@ -560,7 +597,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(C3:I3)</f>
         <v>80</v>
       </c>
     </row>
@@ -593,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J4:J11" si="0">SUM(C4+D4+E4+F4+G4+H4+I4)</f>
         <v>100</v>
       </c>
     </row>
@@ -832,7 +869,36 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
       <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -841,494 +907,492 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12407383-9CC2-42EA-B9EF-9C9CECC58899}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>260</v>
+      </c>
+      <c r="C2" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1">
         <v>9</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>90</v>
+      </c>
+      <c r="I2" s="1">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="K2" s="1">
+        <v>310</v>
+      </c>
+      <c r="L2" s="1">
+        <v>22</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="C3" s="1">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>61</v>
+        <v>1.8</v>
       </c>
       <c r="F3" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="I3" s="1">
         <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="K3" s="1">
-        <v>310</v>
+        <v>140</v>
       </c>
       <c r="L3" s="1">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>300</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>110</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1">
+        <v>155</v>
+      </c>
+      <c r="I4" s="1">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="L4" s="1">
         <v>14</v>
       </c>
-      <c r="E4" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="F4" s="1">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1">
-        <v>150</v>
-      </c>
-      <c r="I4" s="1">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1">
-        <v>140</v>
-      </c>
-      <c r="L4" s="1">
-        <v>16</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1">
-        <v>155</v>
+        <v>285</v>
       </c>
       <c r="I5" s="1">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1">
-        <v>0.85</v>
+        <v>130</v>
       </c>
       <c r="L5" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="F6" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1">
-        <v>285</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="K6" s="1">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="L6" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="C7" s="1">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="F7" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K7" s="1">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="L7" s="1">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>300</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>100</v>
+      </c>
+      <c r="I8" s="1">
         <v>14</v>
       </c>
-      <c r="E8" s="1">
-        <v>270</v>
-      </c>
-      <c r="F8" s="1">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K8" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="L8" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>90</v>
+        <v>450</v>
       </c>
       <c r="C9" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>190</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>140</v>
+      </c>
+      <c r="I9" s="1">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="1">
+        <v>375</v>
+      </c>
+      <c r="L9" s="1">
         <v>14</v>
       </c>
-      <c r="E9" s="1">
-        <v>50</v>
-      </c>
-      <c r="F9" s="1">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1">
-        <v>100</v>
-      </c>
-      <c r="I9" s="1">
-        <v>14</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="1">
-        <v>50</v>
-      </c>
-      <c r="L9" s="1">
-        <v>9</v>
-      </c>
       <c r="M9" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
-        <v>450</v>
-      </c>
-      <c r="C10" s="1">
-        <v>20</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="F10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H10" s="1">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="I10" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="K10" s="1">
-        <v>375</v>
+        <v>300</v>
       </c>
       <c r="L10" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>230</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1">
+        <v>330</v>
+      </c>
+      <c r="F11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>50</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="1">
-        <v>150</v>
-      </c>
-      <c r="F11" s="1">
-        <v>10</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1">
-        <v>150</v>
-      </c>
-      <c r="I11" s="1">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K11" s="1">
-        <v>300</v>
+        <v>210</v>
       </c>
       <c r="L11" s="1">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>230</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="1">
-        <v>330</v>
-      </c>
-      <c r="F12" s="1">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="1">
-        <v>210</v>
-      </c>
-      <c r="L12" s="1">
-        <v>9</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1345,7 +1409,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1382,7 +1446,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>17</v>
@@ -1414,7 +1478,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1478,7 +1542,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -1606,7 +1670,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G10">
         <v>100</v>
@@ -1631,7 +1695,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1641,7 +1705,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1678,7 +1742,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -1704,13 +1768,11 @@
       <c r="J3">
         <v>23.8</v>
       </c>
-      <c r="K3" s="2">
-        <v>3.7755102040816326</v>
-      </c>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1736,9 +1798,7 @@
       <c r="J4">
         <v>16.7</v>
       </c>
-      <c r="K4" s="2">
-        <v>8.9795918367346932</v>
-      </c>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -1768,13 +1828,11 @@
       <c r="J5">
         <v>4.7</v>
       </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>43</v>
@@ -1800,9 +1858,7 @@
       <c r="J6">
         <v>4.7</v>
       </c>
-      <c r="K6" s="2">
-        <v>0.51020408163265307</v>
-      </c>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -1832,9 +1888,7 @@
       <c r="J7">
         <v>16.7</v>
       </c>
-      <c r="K7" s="2">
-        <v>19.897959183673468</v>
-      </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
@@ -1864,9 +1918,7 @@
       <c r="J8">
         <v>2.4</v>
       </c>
-      <c r="K8" s="2">
-        <v>61.734693877551017</v>
-      </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -1896,13 +1948,11 @@
       <c r="J9">
         <v>23.6</v>
       </c>
-      <c r="K9" s="2">
-        <v>5.1020408163265305</v>
-      </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G10">
         <v>33.299999999999997</v>
@@ -1924,20 +1974,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDEDC8C-A34E-4706-BCBA-55B577D110A2}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2">
         <v>1996</v>
       </c>
@@ -1969,9 +2019,9 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1997,13 +2047,16 @@
       <c r="J3">
         <v>15.3</v>
       </c>
-      <c r="K3">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3" s="2">
+        <v>3.7755102040816326</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2029,11 +2082,11 @@
       <c r="J4">
         <v>6.5</v>
       </c>
-      <c r="K4">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4" s="2">
+        <v>8.9795918367346932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2061,13 +2114,13 @@
       <c r="J5">
         <v>0.2</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>33</v>
@@ -2093,11 +2146,11 @@
       <c r="J6">
         <v>0.3</v>
       </c>
-      <c r="K6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K6" s="2">
+        <v>0.51020408163265307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2125,11 +2178,11 @@
       <c r="J7">
         <v>22</v>
       </c>
-      <c r="K7">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7" s="2">
+        <v>19.897959183673468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2157,11 +2210,11 @@
       <c r="J8">
         <v>0.1</v>
       </c>
-      <c r="K8">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" s="2">
+        <v>61.734693877551017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2189,13 +2242,13 @@
       <c r="J9">
         <v>41.1</v>
       </c>
-      <c r="K9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" s="2">
+        <v>5.1020408163265305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G10">
         <v>57.5</v>
@@ -2208,6 +2261,11 @@
       </c>
       <c r="J10">
         <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculated historical relative frequency
</commit_message>
<xml_diff>
--- a/data/clean/aspen_meadow.xlsx
+++ b/data/clean/aspen_meadow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F469D9-A80E-43DD-8CF4-D01A2EF0999B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1717C549-4684-4A46-9B15-8C42557B08BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Ground Cover" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
   <si>
     <t>Shrubs</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>LP-lodgepole pine</t>
+  </si>
+  <si>
+    <t># of time occurred / # of events that can occur</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -909,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12407383-9CC2-42EA-B9EF-9C9CECC58899}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1692,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB20493-A69A-47CD-92E5-3089A7ED8046}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1768,7 +1771,10 @@
       <c r="J3">
         <v>23.8</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2">
+        <f>(5/35)*100</f>
+        <v>14.285714285714285</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -1798,7 +1804,10 @@
       <c r="J4">
         <v>16.7</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2">
+        <f>(9/35)*100</f>
+        <v>25.714285714285712</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -1828,7 +1837,9 @@
       <c r="J5">
         <v>4.7</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -1858,7 +1869,10 @@
       <c r="J6">
         <v>4.7</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2">
+        <f>(1/35)*100</f>
+        <v>2.8571428571428572</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -1888,7 +1902,10 @@
       <c r="J7">
         <v>16.7</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <f>(6/34)*100</f>
+        <v>17.647058823529413</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
@@ -1918,7 +1935,10 @@
       <c r="J8">
         <v>2.4</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <f>(10/35)*100</f>
+        <v>28.571428571428569</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -1948,7 +1968,10 @@
       <c r="J9">
         <v>23.6</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <f>(4/35)*100</f>
+        <v>11.428571428571429</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
@@ -1965,6 +1988,12 @@
       </c>
       <c r="J10">
         <v>7.1</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on aspen meadow graphs
</commit_message>
<xml_diff>
--- a/data/clean/aspen_meadow.xlsx
+++ b/data/clean/aspen_meadow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805D2ABA-7D27-4E74-8B51-23C0A2D8B723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C85514-BE0D-45F5-9844-CD8F4C29DCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Ground Cover" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
   <si>
     <t>Shrubs</t>
   </si>
@@ -1407,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4856CD2D-6C49-49FE-996D-307F8B52A609}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1704,7 +1704,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1718,6 +1718,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -1778,8 +1781,7 @@
         <v>23.8</v>
       </c>
       <c r="K3" s="2">
-        <f>(5/35)*100</f>
-        <v>14.285714285714285</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1811,8 +1813,7 @@
         <v>16.7</v>
       </c>
       <c r="K4" s="2">
-        <f>(9/35)*100</f>
-        <v>25.714285714285712</v>
+        <v>25.7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1876,8 +1877,7 @@
         <v>4.7</v>
       </c>
       <c r="K6" s="2">
-        <f>(1/35)*100</f>
-        <v>2.8571428571428572</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1909,8 +1909,7 @@
         <v>16.7</v>
       </c>
       <c r="K7" s="2">
-        <f>(6/34)*100</f>
-        <v>17.647058823529413</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1942,8 +1941,7 @@
         <v>2.4</v>
       </c>
       <c r="K8" s="2">
-        <f>(10/35)*100</f>
-        <v>28.571428571428569</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1975,8 +1973,7 @@
         <v>23.6</v>
       </c>
       <c r="K9" s="2">
-        <f>(4/35)*100</f>
-        <v>11.428571428571429</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2011,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDEDC8C-A34E-4706-BCBA-55B577D110A2}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2023,6 +2020,9 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>15.3</v>
       </c>
       <c r="K3" s="2">
-        <v>3.7755102040816326</v>
+        <v>3.8</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -2118,7 +2118,7 @@
         <v>6.5</v>
       </c>
       <c r="K4" s="2">
-        <v>8.9795918367346932</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2182,7 +2182,7 @@
         <v>0.3</v>
       </c>
       <c r="K6" s="2">
-        <v>0.51020408163265307</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2214,7 +2214,7 @@
         <v>22</v>
       </c>
       <c r="K7" s="2">
-        <v>19.897959183673468</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2246,7 +2246,7 @@
         <v>0.1</v>
       </c>
       <c r="K8" s="2">
-        <v>61.734693877551017</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2278,7 +2278,7 @@
         <v>41.1</v>
       </c>
       <c r="K9" s="2">
-        <v>5.1020408163265305</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
graph aesthetics, attempt on tree graph
</commit_message>
<xml_diff>
--- a/data/clean/aspen_meadow.xlsx
+++ b/data/clean/aspen_meadow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C85514-BE0D-45F5-9844-CD8F4C29DCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D3CFDC-4D3B-4542-8A72-1E606E1DA9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Ground Cover" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
   <si>
     <t>Shrubs</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Forbs</t>
-  </si>
-  <si>
-    <t>Baby Trees</t>
   </si>
   <si>
     <t>T1-Distance (cm)</t>
@@ -501,7 +498,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -526,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -876,13 +873,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.55000000000000004">
@@ -915,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12407383-9CC2-42EA-B9EF-9C9CECC58899}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -926,40 +923,40 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1374,28 +1371,28 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1420,7 +1417,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>1996</v>
@@ -1719,7 +1716,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>1996</v>
@@ -1996,7 +1993,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2008,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDEDC8C-A34E-4706-BCBA-55B577D110A2}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2021,7 +2018,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>1996</v>
@@ -2298,9 +2295,12 @@
         <v>0.95</v>
       </c>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11" s="2"/>
+    </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>